<commit_message>
schema and plan scheduled checked-in
</commit_message>
<xml_diff>
--- a/documents/timeline/Planning-and-Estimation.xlsx
+++ b/documents/timeline/Planning-and-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE18FCA8-D936-D04B-8E79-372885DDC003}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74601040-27DA-1B47-B4B6-AAC34C8531FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26520" windowHeight="16220" xr2:uid="{0804C6BB-2410-4DC2-BEF2-10EB2FDDC3EB}"/>
   </bookViews>
@@ -1243,10 +1243,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC362AC4-AD3C-47C0-B9B9-5A330255D56D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1287,7 +1288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -2848,7 +2849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>106</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>106</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>106</v>
       </c>
@@ -2881,7 +2882,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -2892,7 +2893,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -2914,7 +2915,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>131</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>131</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>131</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>131</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>131</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>131</v>
       </c>
@@ -3033,7 +3034,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>131</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>131</v>
       </c>
@@ -3069,7 +3070,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>131</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>131</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>131</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>131</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>131</v>
       </c>
@@ -3159,7 +3160,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>131</v>
       </c>
@@ -3177,7 +3178,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>131</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>131</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>131</v>
       </c>
@@ -3231,7 +3232,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>131</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>131</v>
       </c>
@@ -3267,7 +3268,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>131</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>131</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>131</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>131</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>131</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>131</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>131</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>131</v>
       </c>
@@ -3411,7 +3412,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>131</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>131</v>
       </c>
@@ -3447,7 +3448,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>131</v>
       </c>
@@ -3465,7 +3466,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>131</v>
       </c>
@@ -3483,7 +3484,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>131</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>131</v>
       </c>
@@ -3519,7 +3520,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>131</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>131</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>131</v>
       </c>
@@ -3591,7 +3592,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>131</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>131</v>
       </c>
@@ -3645,7 +3646,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>131</v>
       </c>
@@ -3663,7 +3664,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>131</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>131</v>
       </c>
@@ -3699,7 +3700,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>131</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>131</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>131</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>131</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>131</v>
       </c>
@@ -3789,7 +3790,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>131</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>131</v>
       </c>
@@ -3825,7 +3826,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>131</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>131</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>131</v>
       </c>
@@ -3879,7 +3880,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>131</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>131</v>
       </c>
@@ -3915,7 +3916,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>131</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>131</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>131</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>131</v>
       </c>
@@ -3987,7 +3988,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>131</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>131</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>131</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>131</v>
       </c>
@@ -4059,7 +4060,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>131</v>
       </c>
@@ -4077,7 +4078,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>131</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>131</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>131</v>
       </c>
@@ -4131,7 +4132,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>131</v>
       </c>
@@ -4149,7 +4150,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>131</v>
       </c>
@@ -4167,7 +4168,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>131</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>131</v>
       </c>
@@ -4203,7 +4204,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>131</v>
       </c>
@@ -4221,7 +4222,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>131</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>131</v>
       </c>
@@ -4257,7 +4258,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>131</v>
       </c>
@@ -4275,7 +4276,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>131</v>
       </c>
@@ -4293,7 +4294,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>131</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>131</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>131</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>131</v>
       </c>
@@ -4365,7 +4366,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>131</v>
       </c>
@@ -4383,7 +4384,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>131</v>
       </c>
@@ -4401,7 +4402,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>131</v>
       </c>
@@ -4419,7 +4420,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>131</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>131</v>
       </c>
@@ -4455,7 +4456,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>131</v>
       </c>
@@ -4473,7 +4474,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
         <v>157</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
         <v>157</v>
       </c>
@@ -4509,7 +4510,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
         <v>157</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>158</v>
       </c>
@@ -4545,7 +4546,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>158</v>
       </c>
@@ -4563,7 +4564,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>158</v>
       </c>
@@ -4581,7 +4582,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>158</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>158</v>
       </c>
@@ -4617,7 +4618,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>158</v>
       </c>
@@ -4635,7 +4636,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>158</v>
       </c>
@@ -4653,7 +4654,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>158</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>158</v>
       </c>
@@ -4689,7 +4690,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>158</v>
       </c>
@@ -4707,7 +4708,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>158</v>
       </c>
@@ -4725,7 +4726,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>158</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>158</v>
       </c>
@@ -4761,7 +4762,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>158</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>158</v>
       </c>
@@ -4797,7 +4798,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>158</v>
       </c>
@@ -4815,7 +4816,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>158</v>
       </c>
@@ -4833,7 +4834,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>158</v>
       </c>
@@ -4851,7 +4852,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>8</v>
       </c>
@@ -4869,7 +4870,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>8</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>8</v>
       </c>
@@ -4905,7 +4906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>262</v>
       </c>
@@ -4929,7 +4930,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H205" xr:uid="{5CDC9820-C9C6-FA48-9500-4C7CE452EFF0}"/>
+  <autoFilter ref="A1:H205" xr:uid="{5CDC9820-C9C6-FA48-9500-4C7CE452EFF0}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Front-end"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
initial commit for server
</commit_message>
<xml_diff>
--- a/documents/timeline/Planning-and-Estimation.xlsx
+++ b/documents/timeline/Planning-and-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A006A5-9C75-5743-98BA-0D902B5C1701}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D84BD-9E13-1F45-BBBC-083A35DDC552}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26520" windowHeight="16220" activeTab="1" xr2:uid="{0804C6BB-2410-4DC2-BEF2-10EB2FDDC3EB}"/>
   </bookViews>
@@ -5081,7 +5081,7 @@
   <dimension ref="B2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated schema and added raw data details
</commit_message>
<xml_diff>
--- a/documents/timeline/Planning-and-Estimation.xlsx
+++ b/documents/timeline/Planning-and-Estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259DFE88-D617-2848-8125-289368F6D6F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F95712-8D30-E240-9DF8-15275C319784}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26520" windowHeight="16220" xr2:uid="{0804C6BB-2410-4DC2-BEF2-10EB2FDDC3EB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26520" windowHeight="16220" activeTab="1" xr2:uid="{0804C6BB-2410-4DC2-BEF2-10EB2FDDC3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -1322,11 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC362AC4-AD3C-47C0-B9B9-5A330255D56D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:H205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1414,7 +1413,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1435,7 +1434,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1455,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1476,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1549,7 +1548,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1621,7 +1620,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1693,7 +1692,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1783,7 +1782,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1801,7 +1800,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -1873,7 +1872,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
@@ -1927,7 +1926,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -1945,7 +1944,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>11</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -2125,7 +2124,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>11</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>11</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>11</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>11</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>11</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>11</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>11</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>11</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>11</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>11</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>11</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>11</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>11</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>11</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +2520,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>11</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>11</v>
       </c>
@@ -2557,7 +2556,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>11</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>11</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>11</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>11</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>11</v>
       </c>
@@ -2665,7 +2664,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>11</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>11</v>
       </c>
@@ -2701,7 +2700,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>11</v>
       </c>
@@ -2719,7 +2718,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>11</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2754,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>11</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>11</v>
       </c>
@@ -2791,7 +2790,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>11</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>11</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>11</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>11</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>11</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>11</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>11</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>104</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>104</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
         <v>155</v>
       </c>
@@ -4627,7 +4626,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
         <v>155</v>
       </c>
@@ -4645,7 +4644,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
         <v>155</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>156</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>156</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>156</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>156</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>156</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>156</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>156</v>
       </c>
@@ -4789,7 +4788,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>156</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>156</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>156</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>156</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>156</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>156</v>
       </c>
@@ -4897,7 +4896,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>156</v>
       </c>
@@ -4915,7 +4914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>156</v>
       </c>
@@ -4933,7 +4932,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>156</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>156</v>
       </c>
@@ -4969,7 +4968,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>156</v>
       </c>
@@ -4987,7 +4986,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>6</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>6</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>6</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>260</v>
       </c>
@@ -5065,14 +5064,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H205" xr:uid="{5CDC9820-C9C6-FA48-9500-4C7CE452EFF0}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Back-End"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H205" xr:uid="{5CDC9820-C9C6-FA48-9500-4C7CE452EFF0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5080,8 +5074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF36F63-AF2D-AF4F-A1FB-2213F544E376}">
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5198,6 +5192,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>